<commit_message>
chaged psi responsed using function unwrap & fixed nonlinear simulation
</commit_message>
<xml_diff>
--- a/Non linear simulation/Quad.xlsx
+++ b/Non linear simulation/Quad.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{53399D61-7BB0-4879-B4DD-F8CC3460E358}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BA47071C-6A1F-49A6-9999-CA21035CB889}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -583,8 +583,8 @@
         <v>8</v>
       </c>
       <c r="B8" s="4">
-        <f>0*PI()/180</f>
-        <v>0</v>
+        <f>-2*PI()/180</f>
+        <v>-3.4906585039886591E-2</v>
       </c>
       <c r="C8" s="5">
         <v>7</v>
@@ -595,8 +595,8 @@
         <v>9</v>
       </c>
       <c r="B9" s="4">
-        <f>8*PI()/180</f>
-        <v>0.13962634015954636</v>
+        <f>0*PI()/180</f>
+        <v>0</v>
       </c>
       <c r="C9" s="5">
         <v>8</v>

</xml_diff>

<commit_message>
Changed the Nonlinear model
</commit_message>
<xml_diff>
--- a/Non linear simulation/Quad.xlsx
+++ b/Non linear simulation/Quad.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{BA47071C-6A1F-49A6-9999-CA21035CB889}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2B8FE8CB-CDDD-46BE-8FE2-9DD8F9CDF5A5}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -583,8 +583,7 @@
         <v>8</v>
       </c>
       <c r="B8" s="4">
-        <f>-2*PI()/180</f>
-        <v>-3.4906585039886591E-2</v>
+        <v>0</v>
       </c>
       <c r="C8" s="5">
         <v>7</v>

</xml_diff>